<commit_message>
Fix import porducts test
</commit_message>
<xml_diff>
--- a/src/test/resources/product-import.xlsx
+++ b/src/test/resources/product-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BalázsPaulcsik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BalázsPaulcsik\projects\SiliconDreams\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C759F3C8-3DF1-43A9-93AC-BC5C07CEA5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E506D82-8C87-406A-B1CA-F505F6BD2DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2270,15 +2270,9 @@
     <t>110;HUF</t>
   </si>
   <si>
-    <t>Teszt Elek</t>
-  </si>
-  <si>
     <t>Vevő</t>
   </si>
   <si>
-    <t>Teszt Elek|Teszt Blanka</t>
-  </si>
-  <si>
     <t>ProzendaTermék5</t>
   </si>
   <si>
@@ -2286,6 +2280,12 @@
   </si>
   <si>
     <t>termek5</t>
+  </si>
+  <si>
+    <t>Teszt Tamás|Thomas Collins</t>
+  </si>
+  <si>
+    <t>Teszt Tamás</t>
   </si>
 </sst>
 </file>
@@ -2734,9 +2734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
+      <selection pane="bottomLeft" activeCell="CQ8" sqref="CQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3203,7 +3203,7 @@
         <v>125</v>
       </c>
       <c r="CQ3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:100" x14ac:dyDescent="0.35">
@@ -3265,7 +3265,7 @@
         <v>125</v>
       </c>
       <c r="CR4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:100" x14ac:dyDescent="0.35">
@@ -3412,7 +3412,7 @@
         <v>103</v>
       </c>
       <c r="K7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L7" t="s">
         <v>116</v>
@@ -3421,13 +3421,13 @@
         <v>105</v>
       </c>
       <c r="N7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O7" t="s">
         <v>115</v>
       </c>
       <c r="P7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AM7" t="s">
         <v>106</v>
@@ -3439,7 +3439,7 @@
         <v>125</v>
       </c>
       <c r="CQ7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>